<commit_message>
All changes are added
</commit_message>
<xml_diff>
--- a/Bodega Dekorarte/PlantillaSalidas.xlsx
+++ b/Bodega Dekorarte/PlantillaSalidas.xlsx
@@ -685,6 +685,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -746,21 +761,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -769,32 +769,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="48"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thick">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thick">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -829,6 +803,32 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="48"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thick">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1050,9 +1050,9 @@
     <tableColumn id="2" name="IMAGEN" dataDxfId="5"/>
     <tableColumn id="3" name="DESCRIPCION" dataDxfId="4"/>
     <tableColumn id="4" name="ESTADO" dataDxfId="3"/>
-    <tableColumn id="5" name="#" dataDxfId="0"/>
-    <tableColumn id="6" name="VALOR" dataDxfId="2"/>
-    <tableColumn id="7" name="ANOTACIONES" dataDxfId="1"/>
+    <tableColumn id="5" name="#" dataDxfId="2"/>
+    <tableColumn id="6" name="VALOR" dataDxfId="1"/>
+    <tableColumn id="7" name="ANOTACIONES" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1324,8 +1324,7 @@
   <dimension ref="B1:H48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="61.5" x14ac:dyDescent="0.25"/>
@@ -1335,7 +1334,7 @@
     <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="1"/>
-    <col min="6" max="6" width="11.42578125" style="43"/>
+    <col min="6" max="6" width="11.42578125" style="22"/>
     <col min="7" max="7" width="12.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.140625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" style="1"/>
@@ -1343,79 +1342,79 @@
   <sheetData>
     <row r="1" spans="2:8" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="93" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="36"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="41"/>
     </row>
     <row r="5" spans="2:8" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="33"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
     </row>
     <row r="6" spans="2:8" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="42"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="47"/>
     </row>
     <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="39"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="44"/>
     </row>
     <row r="8" spans="2:8" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="2:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
@@ -1447,7 +1446,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="8"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="44"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="8"/>
       <c r="H10" s="3"/>
     </row>
@@ -1458,7 +1457,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="44"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3"/>
       <c r="H11" s="7"/>
     </row>
@@ -1469,7 +1468,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="8"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="45"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
@@ -1480,7 +1479,7 @@
       <c r="C13" s="4"/>
       <c r="D13" s="8"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="45"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
@@ -1491,7 +1490,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="44"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
     </row>
@@ -1502,7 +1501,7 @@
       <c r="C15" s="6"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="46"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="9"/>
       <c r="H15" s="11"/>
     </row>
@@ -1513,7 +1512,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="44"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="8"/>
       <c r="H16" s="7"/>
     </row>
@@ -1524,7 +1523,7 @@
       <c r="C17" s="13"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="47"/>
+      <c r="F17" s="26"/>
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
     </row>

</xml_diff>